<commit_message>
made chain cost prop plot
</commit_message>
<xml_diff>
--- a/Vessels_DATA/ALTERNATIVE_PROP_2/23964TEU_LNG_only_ECA_zones_chain.xlsx
+++ b/Vessels_DATA/ALTERNATIVE_PROP_2/23964TEU_LNG_only_ECA_zones_chain.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roeland van Hagen\Documents\Maritieme techniek\1.Master\MT44070 shipping management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evert\Documents\TU-Delft\TIL Master\MT44070 Shipping Management\MT44070_REPO\MT44070_SHIPPING\Vessels_DATA\ALTERNATIVE_PROP_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31089484-E1EA-4439-86AC-139FEE3BC418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE54008-3905-46AA-BB2E-A666BBEA26C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="0" windowWidth="23016" windowHeight="11976" activeTab="3" xr2:uid="{B8047CF6-A80C-42AA-989D-8358C7959F16}"/>
+    <workbookView xWindow="11244" yWindow="0" windowWidth="11892" windowHeight="12228" xr2:uid="{B8047CF6-A80C-42AA-989D-8358C7959F16}"/>
   </bookViews>
   <sheets>
     <sheet name="CostChain_TwoNuts" sheetId="1" r:id="rId1"/>
@@ -1026,7 +1026,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1044,7 +1044,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1138,7 +1138,7 @@
                   <c:v>1085.7482038294047</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1085.7482038294047</c:v>
+                  <c:v>1085.7482038293999</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1085.7482038294047</c:v>
@@ -1288,7 +1288,7 @@
                   <c:v>1146.3965994494508</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1180.0923218084217</c:v>
+                  <c:v>1180.0923218084199</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1199.231562528804</c:v>
@@ -1363,7 +1363,7 @@
                   <c:v>408.11990845501651</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>381.86848641687573</c:v>
+                  <c:v>381.86848641687601</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>462.74296735146476</c:v>
@@ -1438,7 +1438,7 @@
                   <c:v>423.65886054340342</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>390.61684209720886</c:v>
+                  <c:v>390.61684209720897</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>406.67473658448711</c:v>
@@ -1546,7 +1546,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2049,16 +2049,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>66040</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2324100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>20320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>132080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2128,7 +2128,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2446,7 +2446,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D2E878-2CD8-43EB-9658-FCFB8D281641}">
   <dimension ref="B2:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I11" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2963,22 +2965,22 @@
         <v>22</v>
       </c>
       <c r="I19" s="2">
-        <v>1085.7482038294047</v>
+        <v>1085.7482038293999</v>
       </c>
       <c r="J19" s="2">
         <v>99.652513410564595</v>
       </c>
       <c r="K19" s="2">
-        <v>1180.0923218084217</v>
+        <v>1180.0923218084199</v>
       </c>
       <c r="L19" s="2">
-        <v>381.86848641687573</v>
+        <v>381.86848641687601</v>
       </c>
       <c r="M19" s="2">
-        <v>390.61684209720886</v>
+        <v>390.61684209720897</v>
       </c>
       <c r="N19" s="2">
-        <v>3137.9783675624758</v>
+        <v>3137.9783675624799</v>
       </c>
     </row>
     <row r="20" spans="4:14" x14ac:dyDescent="0.3">
@@ -11803,7 +11805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2470F263-2DD9-4577-A3FE-E4682C3B8CD7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>